<commit_message>
Revised the total sales to indicate the month of December
</commit_message>
<xml_diff>
--- a/Deliverables/Incomplete/Deliverable_1_Grocery_Profiling.xlsx
+++ b/Deliverables/Incomplete/Deliverable_1_Grocery_Profiling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSCode Projects\DW_Grocery_DataMart_RegionC\Deliverables\Incomplete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE097FD4-7347-430A-AD8D-0E6935B356F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E474AA3C-F9B4-44C4-96E9-C467D1630FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
     <t>Combined</t>
   </si>
   <si>
-    <t>Total Sales</t>
+    <t>Total Sales (December)</t>
   </si>
 </sst>
 </file>
@@ -392,7 +392,7 @@
   <dimension ref="B2:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Provided a good starting point for Nikita
</commit_message>
<xml_diff>
--- a/Deliverables/Incomplete/Deliverable_1_Grocery_Profiling.xlsx
+++ b/Deliverables/Incomplete/Deliverable_1_Grocery_Profiling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSCode Projects\DW_Grocery_DataMart_RegionC\Deliverables\Incomplete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E474AA3C-F9B4-44C4-96E9-C467D1630FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F88A58-9DAA-42A6-B818-B0388A62D44F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +82,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -103,14 +113,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -392,7 +405,7 @@
   <dimension ref="B2:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -402,8 +415,11 @@
     <col min="3" max="3" width="12.77734375" customWidth="1"/>
     <col min="4" max="4" width="5.77734375" customWidth="1"/>
     <col min="5" max="5" width="2.77734375" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2.77734375" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="2.77734375" customWidth="1"/>
+    <col min="14" max="14" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.3">
@@ -424,6 +440,15 @@
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="F3" s="2">
+        <v>5573872.9800000004</v>
+      </c>
+      <c r="J3" s="2">
+        <v>3928780.47</v>
+      </c>
+      <c r="N3" s="2">
+        <v>400321.54</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
@@ -433,6 +458,15 @@
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="F5">
+        <v>32750</v>
+      </c>
+      <c r="J5">
+        <v>33382</v>
+      </c>
+      <c r="N5">
+        <v>34141</v>
+      </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">

</xml_diff>

<commit_message>
Fleshed out format for Excel
</commit_message>
<xml_diff>
--- a/Deliverables/Incomplete/Deliverable_1_Grocery_Profiling.xlsx
+++ b/Deliverables/Incomplete/Deliverable_1_Grocery_Profiling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSCode Projects\DW_Grocery_DataMart_RegionC\Deliverables\Incomplete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F88A58-9DAA-42A6-B818-B0388A62D44F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2E6E49-AFFB-4EA3-84C8-F91357D4C52D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>Combined Customer Count (December)</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Total Sales (December)</t>
+  </si>
+  <si>
+    <t>Rank</t>
   </si>
 </sst>
 </file>
@@ -104,12 +107,120 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -117,10 +228,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -402,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:N9"/>
+  <dimension ref="B1:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -422,40 +544,53 @@
     <col min="14" max="14" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B2" s="1"/>
-      <c r="C2" t="s">
+    <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="2"/>
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J2" t="s">
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="N2" t="s">
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+      <c r="O2" s="4"/>
+      <c r="P2" s="5"/>
+    </row>
+    <row r="3" spans="2:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>5573872.9800000004</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="1">
         <v>3928780.47</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="1">
         <v>400321.54</v>
       </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="1" t="s">
+      <c r="P3" s="9"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B4" s="7"/>
+      <c r="P4" s="10"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="F5">
@@ -467,9 +602,22 @@
       <c r="N5">
         <v>34141</v>
       </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
+      <c r="P5" s="10"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B6" s="8"/>
+      <c r="P6" s="10"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B7" s="8"/>
+      <c r="P7" s="10"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B8" s="8"/>
+      <c r="P8" s="10"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B9" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C9" t="s">
@@ -478,7 +626,215 @@
       <c r="D9" t="s">
         <v>3</v>
       </c>
-    </row>
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" t="s">
+        <v>9</v>
+      </c>
+      <c r="N9" t="s">
+        <v>3</v>
+      </c>
+      <c r="O9" t="s">
+        <v>9</v>
+      </c>
+      <c r="P9" s="10"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B10" s="8" t="str">
+        <f>_xlfn.CONCAT("SKU", " ", (ROW() - 9))</f>
+        <v>SKU 1</v>
+      </c>
+      <c r="P10" s="10"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B11" s="8" t="str">
+        <f t="shared" ref="B11:B33" si="0">_xlfn.CONCAT("SKU", " ", (ROW() - 9))</f>
+        <v>SKU 2</v>
+      </c>
+      <c r="P11" s="10"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B12" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 3</v>
+      </c>
+      <c r="P12" s="10"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B13" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 4</v>
+      </c>
+      <c r="P13" s="10"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B14" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 5</v>
+      </c>
+      <c r="P14" s="10"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B15" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 6</v>
+      </c>
+      <c r="P15" s="10"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B16" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 7</v>
+      </c>
+      <c r="P16" s="10"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B17" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 8</v>
+      </c>
+      <c r="P17" s="10"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B18" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 9</v>
+      </c>
+      <c r="P18" s="10"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B19" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 10</v>
+      </c>
+      <c r="P19" s="10"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B20" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 11</v>
+      </c>
+      <c r="P20" s="10"/>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B21" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 12</v>
+      </c>
+      <c r="P21" s="10"/>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B22" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 13</v>
+      </c>
+      <c r="P22" s="10"/>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B23" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 14</v>
+      </c>
+      <c r="P23" s="10"/>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B24" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 15</v>
+      </c>
+      <c r="P24" s="10"/>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B25" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 16</v>
+      </c>
+      <c r="P25" s="10"/>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B26" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 17</v>
+      </c>
+      <c r="P26" s="10"/>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B27" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 18</v>
+      </c>
+      <c r="P27" s="10"/>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B28" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 19</v>
+      </c>
+      <c r="P28" s="10"/>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B29" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 20</v>
+      </c>
+      <c r="P29" s="10"/>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B30" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 21</v>
+      </c>
+      <c r="P30" s="10"/>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B31" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 22</v>
+      </c>
+      <c r="P31" s="10"/>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B32" s="8" t="str">
+        <f>_xlfn.CONCAT("SKU", " ", (ROW() - 9))</f>
+        <v>SKU 23</v>
+      </c>
+      <c r="P32" s="10"/>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B33" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 24</v>
+      </c>
+      <c r="P33" s="10"/>
+    </row>
+    <row r="34" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="11" t="str">
+        <f>_xlfn.CONCAT("SKU", " ", (ROW() - 9))</f>
+        <v>SKU 25</v>
+      </c>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12"/>
+      <c r="N34" s="12"/>
+      <c r="O34" s="12"/>
+      <c r="P34" s="13"/>
+    </row>
+    <row r="35" spans="2:16" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Started populating the Grocery Profiling Excel by hand
</commit_message>
<xml_diff>
--- a/Deliverables/Incomplete/Deliverable_1_Grocery_Profiling.xlsx
+++ b/Deliverables/Incomplete/Deliverable_1_Grocery_Profiling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSCode Projects\DW_Grocery_DataMart_RegionC\Deliverables\Incomplete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29B3746-F679-413C-B5B9-E64CCA2FFE4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CC588A-3F94-4C11-8D29-479DE709E90C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Before" sheetId="1" r:id="rId1"/>
@@ -294,7 +294,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -309,6 +309,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -591,719 +592,662 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:P35"/>
+  <dimension ref="B1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="D8" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.77734375" customWidth="1"/>
     <col min="2" max="2" width="35.44140625" customWidth="1"/>
-    <col min="3" max="3" width="34.6640625" customWidth="1"/>
-    <col min="4" max="4" width="5.77734375" customWidth="1"/>
-    <col min="5" max="5" width="2.77734375" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.77734375" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.77734375" customWidth="1"/>
-    <col min="14" max="14" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="34.6640625" customWidth="1"/>
+    <col min="5" max="5" width="5.77734375" customWidth="1"/>
+    <col min="6" max="6" width="2.77734375" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.77734375" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.77734375" customWidth="1"/>
+    <col min="15" max="15" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:17" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="3"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4"/>
+      <c r="G2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="4"/>
+      <c r="K2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="4"/>
+      <c r="O2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="4"/>
-      <c r="P2" s="5"/>
-    </row>
-    <row r="3" spans="2:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="P2" s="4"/>
+      <c r="Q2" s="5"/>
+    </row>
+    <row r="3" spans="2:17" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="1">
+      <c r="C3" s="14"/>
+      <c r="G3" s="1">
         <v>5573872.9800000004</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <v>3928780.47</v>
       </c>
-      <c r="N3" s="1">
+      <c r="O3" s="1">
         <v>400321.54</v>
       </c>
-      <c r="P3" s="9"/>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="Q3" s="9"/>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B4" s="7"/>
-      <c r="P4" s="10"/>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C4" s="14"/>
+      <c r="Q4" s="10"/>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F5">
+      <c r="C5" s="14"/>
+      <c r="G5">
         <v>32750</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>33382</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>34141</v>
       </c>
-      <c r="P5" s="10"/>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="Q5" s="10"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
-      <c r="P6" s="10"/>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C6" s="15"/>
+      <c r="Q6" s="10"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="8"/>
-      <c r="P7" s="10"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C7" s="15"/>
+      <c r="Q7" s="10"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="8"/>
-      <c r="P8" s="10"/>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C8" s="15"/>
+      <c r="Q8" s="10"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B9" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="14"/>
+      <c r="D9" t="s">
         <v>2</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>3</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>3</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>9</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>3</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>9</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>3</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>9</v>
       </c>
-      <c r="P9" s="10"/>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="Q9" s="10"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="str">
         <f>_xlfn.CONCAT("SKU", " ", (ROW() - 9))</f>
         <v>SKU 1</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10">
+        <v>42359001</v>
+      </c>
+      <c r="D10" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="14">
+      <c r="E10">
         <v>7871</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="10"/>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <v>3746</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>3799</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="10"/>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B11" s="8" t="str">
         <f t="shared" ref="B11:B33" si="0">_xlfn.CONCAT("SKU", " ", (ROW() - 9))</f>
         <v>SKU 2</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11">
+        <v>42356001</v>
+      </c>
+      <c r="D11" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="14">
+      <c r="E11">
         <v>7776</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="10"/>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <v>3691</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="K11">
+        <v>3788</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="10"/>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="str">
         <f t="shared" si="0"/>
         <v>SKU 3</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12">
+        <v>42360001</v>
+      </c>
+      <c r="D12" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="14">
+      <c r="E12">
         <v>7770</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="10"/>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="G12">
+        <v>3682</v>
+      </c>
+      <c r="H12">
+        <v>5</v>
+      </c>
+      <c r="Q12" s="10"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B13" s="8" t="str">
         <f t="shared" si="0"/>
         <v>SKU 4</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13">
+        <v>42355001</v>
+      </c>
+      <c r="D13" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="14">
+      <c r="E13">
         <v>7760</v>
       </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="10"/>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="G13">
+        <v>3733</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="10"/>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B14" s="8" t="str">
         <f t="shared" si="0"/>
         <v>SKU 5</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14">
+        <v>42358001</v>
+      </c>
+      <c r="D14" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="14">
+      <c r="E14">
         <v>7725</v>
       </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="10"/>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="G14">
+        <v>3695</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+      <c r="Q14" s="10"/>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B15" s="8" t="str">
         <f t="shared" si="0"/>
         <v>SKU 6</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15">
+        <v>42357001</v>
+      </c>
+      <c r="D15" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="14">
+      <c r="E15">
         <v>7713</v>
       </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="10"/>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="G15">
+        <v>3680</v>
+      </c>
+      <c r="H15">
+        <v>5</v>
+      </c>
+      <c r="Q15" s="10"/>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="str">
         <f t="shared" si="0"/>
         <v>SKU 7</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16">
+        <v>42311001</v>
+      </c>
+      <c r="D16" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="14">
+      <c r="E16">
         <v>2290</v>
       </c>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="10"/>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <v>1050</v>
+      </c>
+      <c r="H16">
+        <v>8</v>
+      </c>
+      <c r="Q16" s="10"/>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B17" s="8" t="str">
         <f t="shared" si="0"/>
         <v>SKU 8</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17">
+        <v>42314001</v>
+      </c>
+      <c r="D17" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="14">
+      <c r="E17">
         <v>2278</v>
       </c>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="10"/>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="G17">
+        <v>1059</v>
+      </c>
+      <c r="H17">
+        <v>7</v>
+      </c>
+      <c r="Q17" s="10"/>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B18" s="8" t="str">
         <f t="shared" si="0"/>
         <v>SKU 9</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18">
+        <v>42312001</v>
+      </c>
+      <c r="D18" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="14">
+      <c r="E18">
         <v>2267</v>
       </c>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="10"/>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="G18">
+        <v>993</v>
+      </c>
+      <c r="H18">
+        <v>10</v>
+      </c>
+      <c r="Q18" s="10"/>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B19" s="8" t="str">
         <f t="shared" si="0"/>
         <v>SKU 10</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19">
+        <v>42313001</v>
+      </c>
+      <c r="D19" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="14">
+      <c r="E19">
         <v>2266</v>
       </c>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="10"/>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="G19">
+        <v>1009</v>
+      </c>
+      <c r="H19">
+        <v>9</v>
+      </c>
+      <c r="Q19" s="10"/>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B20" s="8" t="str">
         <f t="shared" si="0"/>
         <v>SKU 11</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20">
+        <v>44065001</v>
+      </c>
+      <c r="D20" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="14">
+      <c r="E20">
         <v>1703</v>
       </c>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="10"/>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="G20">
+        <v>890</v>
+      </c>
+      <c r="H20">
+        <v>51</v>
+      </c>
+      <c r="Q20" s="10"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B21" s="8" t="str">
         <f t="shared" si="0"/>
         <v>SKU 12</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21">
+        <v>43675001</v>
+      </c>
+      <c r="D21" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="14">
+      <c r="E21">
         <v>1703</v>
       </c>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="10"/>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="G21">
+        <v>899</v>
+      </c>
+      <c r="H21">
+        <v>15</v>
+      </c>
+      <c r="Q21" s="10"/>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B22" s="8" t="str">
         <f t="shared" si="0"/>
         <v>SKU 13</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22">
+        <v>42650001</v>
+      </c>
+      <c r="D22" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="14">
+      <c r="E22">
         <v>1690</v>
       </c>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="10"/>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="G22">
+        <v>883</v>
+      </c>
+      <c r="H22">
+        <v>71</v>
+      </c>
+      <c r="Q22" s="10"/>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B23" s="8" t="str">
         <f t="shared" si="0"/>
         <v>SKU 14</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23">
+        <v>42835001</v>
+      </c>
+      <c r="D23" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="14">
+      <c r="E23">
         <v>1688</v>
       </c>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="10"/>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="G23">
+        <v>901</v>
+      </c>
+      <c r="H23">
+        <v>27</v>
+      </c>
+      <c r="Q23" s="10"/>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B24" s="8" t="str">
         <f t="shared" si="0"/>
         <v>SKU 15</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24">
+        <v>42756001</v>
+      </c>
+      <c r="D24" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="14">
+      <c r="E24">
         <v>1684</v>
       </c>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="10"/>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="G24">
+        <v>870</v>
+      </c>
+      <c r="H24">
+        <v>82</v>
+      </c>
+      <c r="Q24" s="10"/>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B25" s="8" t="str">
         <f t="shared" si="0"/>
         <v>SKU 16</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25">
+        <v>44148001</v>
+      </c>
+      <c r="D25" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="14">
+      <c r="E25">
         <v>1683</v>
       </c>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="14"/>
-      <c r="P25" s="10"/>
-    </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="G25">
+        <v>832</v>
+      </c>
+      <c r="H25">
+        <v>892</v>
+      </c>
+      <c r="Q25" s="10"/>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B26" s="8" t="str">
         <f t="shared" si="0"/>
         <v>SKU 17</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26">
+        <v>42695001</v>
+      </c>
+      <c r="D26" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="14">
+      <c r="E26">
         <v>1682</v>
       </c>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="10"/>
-    </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="Q26" s="10"/>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B27" s="8" t="str">
         <f t="shared" si="0"/>
         <v>SKU 18</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27">
+        <v>43418001</v>
+      </c>
+      <c r="D27" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="14">
+      <c r="E27">
         <v>1679</v>
       </c>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="10"/>
-    </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="Q27" s="10"/>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B28" s="8" t="str">
         <f t="shared" si="0"/>
         <v>SKU 19</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28">
+        <v>42762001</v>
+      </c>
+      <c r="D28" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="14">
+      <c r="E28">
         <v>1678</v>
       </c>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="10"/>
-    </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="Q28" s="10"/>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B29" s="8" t="str">
         <f t="shared" si="0"/>
         <v>SKU 20</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29">
+        <v>43974001</v>
+      </c>
+      <c r="D29" t="s">
         <v>26</v>
       </c>
-      <c r="D29" s="14">
+      <c r="E29">
         <v>1674</v>
       </c>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
-      <c r="P29" s="10"/>
-    </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="Q29" s="10"/>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B30" s="8" t="str">
         <f t="shared" si="0"/>
         <v>SKU 21</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30">
+        <v>42831001</v>
+      </c>
+      <c r="D30" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="14">
+      <c r="E30">
         <v>1673</v>
       </c>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="14"/>
-      <c r="P30" s="10"/>
-    </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="Q30" s="10"/>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B31" s="8" t="str">
         <f t="shared" si="0"/>
         <v>SKU 22</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31">
+        <v>42838001</v>
+      </c>
+      <c r="D31" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="14">
+      <c r="E31">
         <v>1671</v>
       </c>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="14"/>
-      <c r="P31" s="10"/>
-    </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="Q31" s="10"/>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B32" s="8" t="str">
         <f>_xlfn.CONCAT("SKU", " ", (ROW() - 9))</f>
         <v>SKU 23</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32">
+        <v>44158001</v>
+      </c>
+      <c r="D32" t="s">
         <v>29</v>
       </c>
-      <c r="D32" s="14">
+      <c r="E32">
         <v>1670</v>
       </c>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="14"/>
-      <c r="P32" s="10"/>
-    </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="G32">
+        <v>908</v>
+      </c>
+      <c r="H32">
+        <v>12</v>
+      </c>
+      <c r="Q32" s="10"/>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B33" s="8" t="str">
         <f t="shared" si="0"/>
         <v>SKU 24</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33">
+        <v>43905001</v>
+      </c>
+      <c r="D33" t="s">
         <v>30</v>
       </c>
-      <c r="D33" s="14">
+      <c r="E33">
         <v>1670</v>
       </c>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="14"/>
-      <c r="O33" s="14"/>
-      <c r="P33" s="10"/>
-    </row>
-    <row r="34" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G33">
+        <v>890</v>
+      </c>
+      <c r="H33">
+        <v>71</v>
+      </c>
+      <c r="Q33" s="10"/>
+    </row>
+    <row r="34" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="11" t="str">
         <f>_xlfn.CONCAT("SKU", " ", (ROW() - 9))</f>
         <v>SKU 25</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="12">
+        <v>42988001</v>
+      </c>
+      <c r="D34" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="12">
+      <c r="E34" s="12">
         <v>1669</v>
       </c>
-      <c r="E34" s="12"/>
       <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
+      <c r="G34" s="12">
+        <v>849</v>
+      </c>
+      <c r="H34" s="12">
+        <v>496</v>
+      </c>
       <c r="I34" s="12"/>
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
@@ -1311,9 +1255,10 @@
       <c r="M34" s="12"/>
       <c r="N34" s="12"/>
       <c r="O34" s="12"/>
-      <c r="P34" s="13"/>
-    </row>
-    <row r="35" spans="2:16" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+      <c r="P34" s="12"/>
+      <c r="Q34" s="13"/>
+    </row>
+    <row r="35" spans="2:17" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added completed BEFORE profile before Team 10 was fixed
</commit_message>
<xml_diff>
--- a/Deliverables/Incomplete/Deliverable_1_Grocery_Profiling.xlsx
+++ b/Deliverables/Incomplete/Deliverable_1_Grocery_Profiling.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSCode Projects\DW_Grocery_DataMart_RegionC\Deliverables\Incomplete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CC588A-3F94-4C11-8D29-479DE709E90C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8574FA-63D2-4304-953C-6AB8577BF5F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Before" sheetId="1" r:id="rId1"/>
+    <sheet name="After" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
   <si>
     <t>Combined Customer Count (December)</t>
   </si>
@@ -294,7 +295,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -309,8 +310,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -594,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D8" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -606,9 +606,11 @@
     <col min="4" max="4" width="34.6640625" customWidth="1"/>
     <col min="5" max="5" width="5.77734375" customWidth="1"/>
     <col min="6" max="6" width="2.77734375" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="9" width="8.88671875" customWidth="1"/>
     <col min="10" max="10" width="2.77734375" customWidth="1"/>
-    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" customWidth="1"/>
+    <col min="12" max="13" width="8.88671875" customWidth="1"/>
     <col min="14" max="14" width="2.77734375" customWidth="1"/>
     <col min="15" max="15" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -679,17 +681,14 @@
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
-      <c r="C6" s="15"/>
       <c r="Q6" s="10"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="8"/>
-      <c r="C7" s="15"/>
       <c r="Q7" s="10"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="8"/>
-      <c r="C8" s="15"/>
       <c r="Q8" s="10"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
@@ -697,28 +696,33 @@
         <v>1</v>
       </c>
       <c r="C9" s="14"/>
-      <c r="D9" t="s">
+      <c r="D9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G9" t="s">
+      <c r="F9" s="14"/>
+      <c r="G9" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K9" t="s">
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="O9" t="s">
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="P9" t="s">
+      <c r="P9" s="14" t="s">
         <v>9</v>
       </c>
       <c r="Q9" s="10"/>
@@ -749,6 +753,12 @@
       <c r="L10">
         <v>1</v>
       </c>
+      <c r="O10">
+        <v>52</v>
+      </c>
+      <c r="P10">
+        <v>389</v>
+      </c>
       <c r="Q10" s="10"/>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.3">
@@ -777,6 +787,12 @@
       <c r="L11">
         <v>2</v>
       </c>
+      <c r="O11">
+        <v>39</v>
+      </c>
+      <c r="P11">
+        <v>1860</v>
+      </c>
       <c r="Q11" s="10"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
@@ -799,6 +815,18 @@
       <c r="H12">
         <v>5</v>
       </c>
+      <c r="K12">
+        <v>3783</v>
+      </c>
+      <c r="L12">
+        <v>3</v>
+      </c>
+      <c r="O12">
+        <v>53</v>
+      </c>
+      <c r="P12">
+        <v>464</v>
+      </c>
       <c r="Q12" s="10"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
@@ -821,6 +849,18 @@
       <c r="H13">
         <v>2</v>
       </c>
+      <c r="K13">
+        <v>3742</v>
+      </c>
+      <c r="L13">
+        <v>6</v>
+      </c>
+      <c r="O13">
+        <v>43</v>
+      </c>
+      <c r="P13">
+        <v>1557</v>
+      </c>
       <c r="Q13" s="10"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
@@ -843,6 +883,18 @@
       <c r="H14">
         <v>3</v>
       </c>
+      <c r="K14">
+        <v>3723</v>
+      </c>
+      <c r="L14">
+        <v>5</v>
+      </c>
+      <c r="O14">
+        <v>52</v>
+      </c>
+      <c r="P14">
+        <v>633</v>
+      </c>
       <c r="Q14" s="10"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
@@ -865,6 +917,18 @@
       <c r="H15">
         <v>5</v>
       </c>
+      <c r="K15">
+        <v>3715</v>
+      </c>
+      <c r="L15">
+        <v>4</v>
+      </c>
+      <c r="O15">
+        <v>45</v>
+      </c>
+      <c r="P15">
+        <v>1253</v>
+      </c>
       <c r="Q15" s="10"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
@@ -887,6 +951,18 @@
       <c r="H16">
         <v>8</v>
       </c>
+      <c r="K16">
+        <v>1126</v>
+      </c>
+      <c r="L16">
+        <v>9</v>
+      </c>
+      <c r="O16">
+        <v>39</v>
+      </c>
+      <c r="P16">
+        <v>1896</v>
+      </c>
       <c r="Q16" s="10"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.3">
@@ -909,6 +985,18 @@
       <c r="H17">
         <v>7</v>
       </c>
+      <c r="K17">
+        <v>1096</v>
+      </c>
+      <c r="L17">
+        <v>10</v>
+      </c>
+      <c r="O17">
+        <v>46</v>
+      </c>
+      <c r="P17">
+        <v>990</v>
+      </c>
       <c r="Q17" s="10"/>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.3">
@@ -931,6 +1019,18 @@
       <c r="H18">
         <v>10</v>
       </c>
+      <c r="K18">
+        <v>1159</v>
+      </c>
+      <c r="L18">
+        <v>7</v>
+      </c>
+      <c r="O18">
+        <v>49</v>
+      </c>
+      <c r="P18">
+        <v>990</v>
+      </c>
       <c r="Q18" s="10"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.3">
@@ -953,6 +1053,18 @@
       <c r="H19">
         <v>9</v>
       </c>
+      <c r="K19">
+        <v>1147</v>
+      </c>
+      <c r="L19">
+        <v>8</v>
+      </c>
+      <c r="O19">
+        <v>42</v>
+      </c>
+      <c r="P19">
+        <v>1641</v>
+      </c>
       <c r="Q19" s="10"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.3">
@@ -975,6 +1087,18 @@
       <c r="H20">
         <v>51</v>
       </c>
+      <c r="K20">
+        <v>712</v>
+      </c>
+      <c r="L20">
+        <v>24</v>
+      </c>
+      <c r="O20">
+        <v>58</v>
+      </c>
+      <c r="P20">
+        <v>67</v>
+      </c>
       <c r="Q20" s="10"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.3">
@@ -997,6 +1121,18 @@
       <c r="H21">
         <v>15</v>
       </c>
+      <c r="K21">
+        <v>699</v>
+      </c>
+      <c r="L21">
+        <v>45</v>
+      </c>
+      <c r="O21">
+        <v>48</v>
+      </c>
+      <c r="P21">
+        <v>866</v>
+      </c>
       <c r="Q21" s="10"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.3">
@@ -1019,6 +1155,18 @@
       <c r="H22">
         <v>71</v>
       </c>
+      <c r="K22">
+        <v>710</v>
+      </c>
+      <c r="L22">
+        <v>20</v>
+      </c>
+      <c r="O22">
+        <v>49</v>
+      </c>
+      <c r="P22">
+        <v>866</v>
+      </c>
       <c r="Q22" s="10"/>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.3">
@@ -1041,6 +1189,18 @@
       <c r="H23">
         <v>27</v>
       </c>
+      <c r="K23">
+        <v>683</v>
+      </c>
+      <c r="L23">
+        <v>180</v>
+      </c>
+      <c r="O23">
+        <v>63</v>
+      </c>
+      <c r="P23">
+        <v>27</v>
+      </c>
       <c r="Q23" s="10"/>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.3">
@@ -1063,6 +1223,18 @@
       <c r="H24">
         <v>82</v>
       </c>
+      <c r="K24">
+        <v>687</v>
+      </c>
+      <c r="L24">
+        <v>48</v>
+      </c>
+      <c r="O24">
+        <v>53</v>
+      </c>
+      <c r="P24">
+        <v>191</v>
+      </c>
       <c r="Q24" s="10"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.3">
@@ -1085,6 +1257,18 @@
       <c r="H25">
         <v>892</v>
       </c>
+      <c r="K25">
+        <v>741</v>
+      </c>
+      <c r="L25">
+        <v>11</v>
+      </c>
+      <c r="O25">
+        <v>47</v>
+      </c>
+      <c r="P25">
+        <v>746</v>
+      </c>
       <c r="Q25" s="10"/>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.3">
@@ -1101,6 +1285,24 @@
       <c r="E26">
         <v>1682</v>
       </c>
+      <c r="G26">
+        <v>883</v>
+      </c>
+      <c r="H26">
+        <v>32</v>
+      </c>
+      <c r="K26">
+        <v>693</v>
+      </c>
+      <c r="L26">
+        <v>42</v>
+      </c>
+      <c r="O26">
+        <v>40</v>
+      </c>
+      <c r="P26">
+        <v>1860</v>
+      </c>
       <c r="Q26" s="10"/>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.3">
@@ -1117,6 +1319,24 @@
       <c r="E27">
         <v>1679</v>
       </c>
+      <c r="G27">
+        <v>868</v>
+      </c>
+      <c r="H27">
+        <v>108</v>
+      </c>
+      <c r="K27">
+        <v>705</v>
+      </c>
+      <c r="L27">
+        <v>35</v>
+      </c>
+      <c r="O27">
+        <v>52</v>
+      </c>
+      <c r="P27">
+        <v>552</v>
+      </c>
       <c r="Q27" s="10"/>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.3">
@@ -1133,6 +1353,24 @@
       <c r="E28">
         <v>1678</v>
       </c>
+      <c r="G28">
+        <v>883</v>
+      </c>
+      <c r="H28">
+        <v>51</v>
+      </c>
+      <c r="K28">
+        <v>686</v>
+      </c>
+      <c r="L28">
+        <v>117</v>
+      </c>
+      <c r="O28">
+        <v>54</v>
+      </c>
+      <c r="P28">
+        <v>320</v>
+      </c>
       <c r="Q28" s="10"/>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.3">
@@ -1149,6 +1387,24 @@
       <c r="E29">
         <v>1674</v>
       </c>
+      <c r="G29">
+        <v>883</v>
+      </c>
+      <c r="H29">
+        <v>63</v>
+      </c>
+      <c r="K29">
+        <v>693</v>
+      </c>
+      <c r="L29">
+        <v>48</v>
+      </c>
+      <c r="O29">
+        <v>44</v>
+      </c>
+      <c r="P29">
+        <v>1557</v>
+      </c>
       <c r="Q29" s="10"/>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.3">
@@ -1165,6 +1421,24 @@
       <c r="E30">
         <v>1673</v>
       </c>
+      <c r="G30">
+        <v>861</v>
+      </c>
+      <c r="H30">
+        <v>182</v>
+      </c>
+      <c r="K30">
+        <v>705</v>
+      </c>
+      <c r="L30">
+        <v>24</v>
+      </c>
+      <c r="O30">
+        <v>51</v>
+      </c>
+      <c r="P30">
+        <v>746</v>
+      </c>
       <c r="Q30" s="10"/>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.3">
@@ -1180,6 +1454,24 @@
       </c>
       <c r="E31">
         <v>1671</v>
+      </c>
+      <c r="G31">
+        <v>887</v>
+      </c>
+      <c r="H31">
+        <v>45</v>
+      </c>
+      <c r="K31">
+        <v>685</v>
+      </c>
+      <c r="L31">
+        <v>166</v>
+      </c>
+      <c r="O31">
+        <v>52</v>
+      </c>
+      <c r="P31">
+        <v>389</v>
       </c>
       <c r="Q31" s="10"/>
     </row>
@@ -1203,6 +1495,18 @@
       <c r="H32">
         <v>12</v>
       </c>
+      <c r="K32">
+        <v>653</v>
+      </c>
+      <c r="L32">
+        <v>648</v>
+      </c>
+      <c r="O32">
+        <v>49</v>
+      </c>
+      <c r="P32">
+        <v>866</v>
+      </c>
       <c r="Q32" s="10"/>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.3">
@@ -1224,6 +1528,18 @@
       </c>
       <c r="H33">
         <v>71</v>
+      </c>
+      <c r="K33">
+        <v>676</v>
+      </c>
+      <c r="L33">
+        <v>152</v>
+      </c>
+      <c r="O33">
+        <v>55</v>
+      </c>
+      <c r="P33">
+        <v>191</v>
       </c>
       <c r="Q33" s="10"/>
     </row>
@@ -1248,6 +1564,345 @@
       <c r="H34" s="12">
         <v>496</v>
       </c>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12">
+        <v>716</v>
+      </c>
+      <c r="L34" s="12">
+        <v>14</v>
+      </c>
+      <c r="M34" s="12"/>
+      <c r="N34" s="12"/>
+      <c r="O34" s="12">
+        <v>47</v>
+      </c>
+      <c r="P34" s="12">
+        <v>746</v>
+      </c>
+      <c r="Q34" s="13"/>
+    </row>
+    <row r="35" spans="2:17" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0B1CB71-1363-417F-B130-26B6ABD9790D}">
+  <dimension ref="B1:Q35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.77734375" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="34.6640625" customWidth="1"/>
+    <col min="5" max="5" width="5.77734375" customWidth="1"/>
+    <col min="6" max="6" width="2.77734375" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="10" max="10" width="2.77734375" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" customWidth="1"/>
+    <col min="14" max="14" width="2.77734375" customWidth="1"/>
+    <col min="15" max="15" width="12.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:17" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="2"/>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="5"/>
+    </row>
+    <row r="3" spans="2:17" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="G3" s="1">
+        <v>5573872.9800000004</v>
+      </c>
+      <c r="K3" s="1">
+        <v>3928780.47</v>
+      </c>
+      <c r="O3" s="1">
+        <v>400321.54</v>
+      </c>
+      <c r="Q3" s="9"/>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B4" s="7"/>
+      <c r="C4" s="14"/>
+      <c r="Q4" s="10"/>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B5" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="G5">
+        <v>32750</v>
+      </c>
+      <c r="K5">
+        <v>33382</v>
+      </c>
+      <c r="O5">
+        <v>34141</v>
+      </c>
+      <c r="Q5" s="10"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B6" s="8"/>
+      <c r="Q6" s="10"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B7" s="8"/>
+      <c r="Q7" s="10"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B8" s="8"/>
+      <c r="Q8" s="10"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="L9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="P9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q9" s="10"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B10" s="8" t="str">
+        <f>_xlfn.CONCAT("SKU", " ", (ROW() - 9))</f>
+        <v>SKU 1</v>
+      </c>
+      <c r="Q10" s="10"/>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B11" s="8" t="str">
+        <f t="shared" ref="B11:B33" si="0">_xlfn.CONCAT("SKU", " ", (ROW() - 9))</f>
+        <v>SKU 2</v>
+      </c>
+      <c r="Q11" s="10"/>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B12" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 3</v>
+      </c>
+      <c r="Q12" s="10"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B13" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 4</v>
+      </c>
+      <c r="Q13" s="10"/>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B14" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 5</v>
+      </c>
+      <c r="Q14" s="10"/>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B15" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 6</v>
+      </c>
+      <c r="Q15" s="10"/>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B16" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 7</v>
+      </c>
+      <c r="Q16" s="10"/>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B17" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 8</v>
+      </c>
+      <c r="Q17" s="10"/>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B18" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 9</v>
+      </c>
+      <c r="Q18" s="10"/>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B19" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 10</v>
+      </c>
+      <c r="Q19" s="10"/>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B20" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 11</v>
+      </c>
+      <c r="Q20" s="10"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B21" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 12</v>
+      </c>
+      <c r="Q21" s="10"/>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B22" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 13</v>
+      </c>
+      <c r="Q22" s="10"/>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B23" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 14</v>
+      </c>
+      <c r="Q23" s="10"/>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B24" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 15</v>
+      </c>
+      <c r="Q24" s="10"/>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B25" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 16</v>
+      </c>
+      <c r="Q25" s="10"/>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B26" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 17</v>
+      </c>
+      <c r="Q26" s="10"/>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B27" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 18</v>
+      </c>
+      <c r="Q27" s="10"/>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B28" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 19</v>
+      </c>
+      <c r="Q28" s="10"/>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B29" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 20</v>
+      </c>
+      <c r="Q29" s="10"/>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B30" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 21</v>
+      </c>
+      <c r="Q30" s="10"/>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B31" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 22</v>
+      </c>
+      <c r="Q31" s="10"/>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B32" s="8" t="str">
+        <f>_xlfn.CONCAT("SKU", " ", (ROW() - 9))</f>
+        <v>SKU 23</v>
+      </c>
+      <c r="Q32" s="10"/>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B33" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SKU 24</v>
+      </c>
+      <c r="Q33" s="10"/>
+    </row>
+    <row r="34" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="11" t="str">
+        <f>_xlfn.CONCAT("SKU", " ", (ROW() - 9))</f>
+        <v>SKU 25</v>
+      </c>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
       <c r="I34" s="12"/>
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
@@ -1261,6 +1916,5 @@
     <row r="35" spans="2:17" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>